<commit_message>
Update to excel data set and coefficients calculated using kp and kag
</commit_message>
<xml_diff>
--- a/Ag_kinetics.xlsx
+++ b/Ag_kinetics.xlsx
@@ -5,17 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luise\iCloudDrive\Ennova\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luise\iCloudDrive\Ennova\P&amp;A kinetics tuning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A05866-6C1D-43D1-A5F2-F220522BD433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5880B87-BF7B-43A1-95CE-2596AC7DF8B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{85EE5AE4-3DA7-4426-97B8-6903418DBB70}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{85EE5AE4-3DA7-4426-97B8-6903418DBB70}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="2" r:id="rId1"/>
     <sheet name="Set1" sheetId="1" r:id="rId2"/>
     <sheet name="Set2" sheetId="3" r:id="rId3"/>
+    <sheet name="Set3" sheetId="4" r:id="rId4"/>
+    <sheet name="Set4" sheetId="5" r:id="rId5"/>
+    <sheet name="Set5" sheetId="6" r:id="rId6"/>
+    <sheet name="Set6" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
   <si>
     <t>time (min)</t>
   </si>
@@ -61,11 +65,17 @@
   <si>
     <t>PC-003</t>
   </si>
+  <si>
+    <t>ceq</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -83,12 +93,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -103,9 +119,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,31 +476,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5717BD04-681A-47BF-99CC-63688E75A42A}">
-  <dimension ref="B1:C42"/>
+  <dimension ref="B1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>0.85828150950348459</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>1.2</v>
       </c>
@@ -491,7 +514,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2.2000000000000002</v>
       </c>
@@ -499,7 +522,7 @@
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>3.2</v>
       </c>
@@ -507,7 +530,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>4.2</v>
       </c>
@@ -515,7 +538,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>5.8</v>
       </c>
@@ -523,7 +546,7 @@
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>6.8</v>
       </c>
@@ -531,7 +554,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>8.8000000000000007</v>
       </c>
@@ -539,7 +562,7 @@
         <v>4.9000000000000002E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>10</v>
       </c>
@@ -547,7 +570,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>12</v>
       </c>
@@ -555,7 +578,7 @@
         <v>6.7000000000000004E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>14</v>
       </c>
@@ -563,7 +586,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>17</v>
       </c>
@@ -571,7 +594,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>20</v>
       </c>
@@ -579,7 +602,7 @@
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>23</v>
       </c>
@@ -587,7 +610,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>27</v>
       </c>
@@ -810,31 +833,37 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38A111BB-A23C-48E8-9875-888A70D3D01B}">
-  <dimension ref="B1:C38"/>
+  <dimension ref="B1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>0.8334033946256143</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>1.2</v>
       </c>
@@ -842,7 +871,7 @@
         <v>1.9509430993236314E-2</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2.21</v>
       </c>
@@ -850,7 +879,7 @@
         <v>2.7243526851269281E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>2.7149999999999999</v>
       </c>
@@ -858,7 +887,7 @@
         <v>3.6092447337487177E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>2.7151000000000001</v>
       </c>
@@ -866,7 +895,7 @@
         <v>4.7728429394167389E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>3.7249999999999996</v>
       </c>
@@ -874,7 +903,7 @@
         <v>5.7274115273000872E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>5.24</v>
       </c>
@@ -882,7 +911,7 @@
         <v>6.6192712298480338E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>6.7560000000000002</v>
       </c>
@@ -890,7 +919,7 @@
         <v>7.504163278469822E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>8.270999999999999</v>
       </c>
@@ -898,7 +927,7 @@
         <v>8.5005377899101051E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>11.301</v>
       </c>
@@ -906,7 +935,7 @@
         <v>9.62929772594735E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>14.331</v>
       </c>
@@ -914,7 +943,7 @@
         <v>0.10549028044199918</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>18.372</v>
       </c>
@@ -922,7 +951,7 @@
         <v>0.11266696398593969</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>23.422000000000001</v>
       </c>
@@ -930,7 +959,7 @@
         <v>0.12158556101141911</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>28.977999999999998</v>
       </c>
@@ -938,7 +967,7 @@
         <v>0.12771709646643623</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>35.038000000000004</v>
       </c>
@@ -1120,6 +1149,1178 @@
       </c>
       <c r="C38">
         <v>0.16659660537438575</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157ECD7F-F4ED-435B-B519-EAB347D4C132}">
+  <dimension ref="B1:D35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0.84863284550247642</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>0.505</v>
+      </c>
+      <c r="C3" s="2">
+        <v>6.9062154215709208E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>2.02</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.3171647968975487E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>3.03</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.844030715656567E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>4.04</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2.5773711160914176E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>5.556</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3.2751124679614697E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>7.0709999999999997</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3.8660566741371277E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>9.0909999999999993</v>
+      </c>
+      <c r="C9" s="2">
+        <v>4.5637980260071806E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>10.606</v>
+      </c>
+      <c r="C10" s="2">
+        <v>5.1618620418957963E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>13.635999999999999</v>
+      </c>
+      <c r="C11" s="2">
+        <v>5.7884052966362516E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>15.151999999999999</v>
+      </c>
+      <c r="C12" s="2">
+        <v>6.4505475999415043E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>20.202000000000002</v>
+      </c>
+      <c r="C13" s="2">
+        <v>7.4330813403299445E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>25.253</v>
+      </c>
+      <c r="C14" s="2">
+        <v>8.408495271005427E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>30.808</v>
+      </c>
+      <c r="C15" s="2">
+        <v>9.1133564325884389E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>39.899000000000001</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.10337963703217513</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>48.99</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.11000106006522765</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>58.081000000000003</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.11669368119540977</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>70.706999999999994</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.12367109471411034</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>85.858999999999995</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.12972293297012608</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>103.03</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.13427961118642032</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>123.232</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.13855149701419608</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>148.99</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.14282338284197191</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>176.26300000000001</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.14467453336734148</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>209.596</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.14759365534965496</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>226.768</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.14866162680659895</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>250.505</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.14944480587502448</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>273.73700000000002</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.14987199445780205</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>303.02999999999997</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.15101116401187561</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>321.71699999999998</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.15143835259465319</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>340.90899999999999</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.15186554117743081</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>357.57600000000002</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0.15158074878891237</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>371.71699999999998</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.151651946886042</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>389.39400000000001</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.15172314498317158</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>397.47500000000002</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0.15136715449752361</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C61FE8E4-D459-4246-B04F-D0D9F84D37E9}">
+  <dimension ref="B1:D33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0.83722655227512</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1.3522495878160609E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>2.4710000000000001</v>
+      </c>
+      <c r="C4">
+        <v>2.4024008634604473E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>3.4510000000000001</v>
+      </c>
+      <c r="C5">
+        <v>3.1936107286719709E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>4.9220000000000006</v>
+      </c>
+      <c r="C6">
+        <v>3.9488565091011521E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>6.3920000000000003</v>
+      </c>
+      <c r="C7">
+        <v>4.9414652490937946E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>8.843</v>
+      </c>
+      <c r="C8">
+        <v>5.7974104669135336E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>10.314</v>
+      </c>
+      <c r="C9">
+        <v>6.7252838542979573E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>13.744999999999999</v>
+      </c>
+      <c r="C10">
+        <v>7.5812290721176984E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>18.646999999999998</v>
+      </c>
+      <c r="C11">
+        <v>8.7105013342832383E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>22.568999999999999</v>
+      </c>
+      <c r="C12">
+        <v>9.4297830299300778E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>28.940999999999999</v>
+      </c>
+      <c r="C13">
+        <v>0.10429584586879187</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>34.823999999999998</v>
+      </c>
+      <c r="C14">
+        <v>0.11285529804698927</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>45.118000000000002</v>
+      </c>
+      <c r="C15">
+        <v>0.12177439107301008</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>50.51</v>
+      </c>
+      <c r="C16">
+        <v>0.12796021365557292</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>64.724999999999994</v>
+      </c>
+      <c r="C17">
+        <v>0.13594424047725284</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>88.745000000000005</v>
+      </c>
+      <c r="C18">
+        <v>0.14594225604674393</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>108.35299999999999</v>
+      </c>
+      <c r="C19">
+        <v>0.15184036595104802</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>133.84299999999999</v>
+      </c>
+      <c r="C20">
+        <v>0.15565255893797625</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>157.37299999999999</v>
+      </c>
+      <c r="C21">
+        <v>0.15845775755099895</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>176</v>
+      </c>
+      <c r="C22">
+        <v>0.16025596179011603</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>195.11799999999999</v>
+      </c>
+      <c r="C23">
+        <v>0.16032788995968072</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>214.72499999999999</v>
+      </c>
+      <c r="C24">
+        <v>0.16111909982489225</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>246.09800000000001</v>
+      </c>
+      <c r="C25">
+        <v>0.16119102799445692</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>271.58800000000002</v>
+      </c>
+      <c r="C26">
+        <v>0.16198223785966845</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>290.21600000000001</v>
+      </c>
+      <c r="C27">
+        <v>0.16234187870749184</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>310.80399999999997</v>
+      </c>
+      <c r="C28">
+        <v>0.16277344772488</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>329.92200000000003</v>
+      </c>
+      <c r="C29">
+        <v>0.1628453758944447</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>346.09800000000001</v>
+      </c>
+      <c r="C30">
+        <v>0.16291730406400934</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>364.23500000000001</v>
+      </c>
+      <c r="C31">
+        <v>0.16298923223357403</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>377.471</v>
+      </c>
+      <c r="C32">
+        <v>0.16298923223357403</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>398.05900000000003</v>
+      </c>
+      <c r="C33">
+        <v>0.16277344772488</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E6FB475-3B1D-4313-A414-B5EEBD6943DB}">
+  <dimension ref="B1:D34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0.85321571075835068</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>6.9300468049799269E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>3.9409999999999998</v>
+      </c>
+      <c r="C4">
+        <v>1.518712384921133E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>4.9220000000000006</v>
+      </c>
+      <c r="C5">
+        <v>2.0790140414939789E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>6.3920000000000003</v>
+      </c>
+      <c r="C6">
+        <v>2.6393156980668232E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>8.843</v>
+      </c>
+      <c r="C7">
+        <v>3.310203207910626E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>10.314</v>
+      </c>
+      <c r="C8">
+        <v>3.9073668155737894E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>13.744999999999999</v>
+      </c>
+      <c r="C9">
+        <v>4.7109573493427384E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>18.157</v>
+      </c>
+      <c r="C10">
+        <v>5.6325061266007073E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>22.568999999999999</v>
+      </c>
+      <c r="C11">
+        <v>6.3992347092793403E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>29.431000000000001</v>
+      </c>
+      <c r="C12">
+        <v>7.3502730474095626E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>38.255000000000003</v>
+      </c>
+      <c r="C13">
+        <v>8.5151107018636374E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>45.607999999999997</v>
+      </c>
+      <c r="C14">
+        <v>9.2228601627977566E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>53.451000000000001</v>
+      </c>
+      <c r="C15">
+        <v>0.10137036549837664</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>64.724999999999994</v>
+      </c>
+      <c r="C16">
+        <v>0.10911137522734357</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>77.471000000000004</v>
+      </c>
+      <c r="C17">
+        <v>0.11618886983668475</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>90.215999999999994</v>
+      </c>
+      <c r="C18">
+        <v>0.12149699079369065</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>107.863</v>
+      </c>
+      <c r="C19">
+        <v>0.12783724638122551</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>127.961</v>
+      </c>
+      <c r="C20">
+        <v>0.13248185221860567</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>146.09800000000001</v>
+      </c>
+      <c r="C21">
+        <v>0.13506218879492798</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>165.21600000000001</v>
+      </c>
+      <c r="C22">
+        <v>0.13823231658869539</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>184.333</v>
+      </c>
+      <c r="C23">
+        <v>0.14110754877374024</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>200.02</v>
+      </c>
+      <c r="C24">
+        <v>0.14258202681735296</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>226.49</v>
+      </c>
+      <c r="C25">
+        <v>0.14479374388277214</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>240.70599999999999</v>
+      </c>
+      <c r="C26">
+        <v>0.14553098290457853</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>257.863</v>
+      </c>
+      <c r="C27">
+        <v>0.1456047068067591</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>277.96100000000001</v>
+      </c>
+      <c r="C28">
+        <v>0.14634194582856552</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>297.56900000000002</v>
+      </c>
+      <c r="C29">
+        <v>0.14641566973074613</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>317.66699999999997</v>
+      </c>
+      <c r="C30">
+        <v>0.14685801314382999</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>339.23500000000001</v>
+      </c>
+      <c r="C31">
+        <v>0.14730035655691381</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>361.29399999999998</v>
+      </c>
+      <c r="C32">
+        <v>0.14737408045909442</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>380.90199999999999</v>
+      </c>
+      <c r="C33">
+        <v>0.14707918485037186</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>398.05900000000003</v>
+      </c>
+      <c r="C34">
+        <v>0.14678428924164932</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C99278E9-CACF-48CD-A01A-0599567D5678}">
+  <dimension ref="B1:D34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0.85843032728620305</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>1.7333333333333334</v>
+      </c>
+      <c r="C3">
+        <v>7.8440308802530043E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>5.1643333333333334</v>
+      </c>
+      <c r="C4">
+        <v>1.1539776198833744E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>8.1063333333333336</v>
+      </c>
+      <c r="C5">
+        <v>1.5537215012808832E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>10.557333333333332</v>
+      </c>
+      <c r="C6">
+        <v>2.1269391425301407E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>12.517333333333333</v>
+      </c>
+      <c r="C7">
+        <v>2.5945640603913769E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>14.968333333333334</v>
+      </c>
+      <c r="C8">
+        <v>3.137612352101201E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>19.870333333333335</v>
+      </c>
+      <c r="C9">
+        <v>3.7862533671990453E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>25.262333333333334</v>
+      </c>
+      <c r="C10">
+        <v>4.6460798290729327E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>31.145333333333333</v>
+      </c>
+      <c r="C11">
+        <v>5.5134486283316769E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>35.557333333333332</v>
+      </c>
+      <c r="C12">
+        <v>6.3732750902055629E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>44.870333333333335</v>
+      </c>
+      <c r="C13">
+        <v>7.6026760839375249E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>54.674333333333337</v>
+      </c>
+      <c r="C14">
+        <v>8.5002142327357047E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>64.968333333333334</v>
+      </c>
+      <c r="C15">
+        <v>9.3675830319944489E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>78.204333333333338</v>
+      </c>
+      <c r="C16">
+        <v>0.1015952845740461</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>89.968333333333334</v>
+      </c>
+      <c r="C17">
+        <v>0.10959016220199626</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>103.20433333333334</v>
+      </c>
+      <c r="C18">
+        <v>0.11675538271761197</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>121.34133333333334</v>
+      </c>
+      <c r="C19">
+        <v>0.12188417213931585</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>137.51733333333331</v>
+      </c>
+      <c r="C20">
+        <v>0.1258816109532909</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>150.75333333333333</v>
+      </c>
+      <c r="C21">
+        <v>0.12950193289802309</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>175.26233333333332</v>
+      </c>
+      <c r="C22">
+        <v>0.13319767821660383</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>197.81133333333332</v>
+      </c>
+      <c r="C23">
+        <v>0.1361391897966987</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>216.92933333333332</v>
+      </c>
+      <c r="C24">
+        <v>0.13840189101215636</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>237.02733333333333</v>
+      </c>
+      <c r="C25">
+        <v>0.13991035848912806</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>256.14533333333333</v>
+      </c>
+      <c r="C26">
+        <v>0.13998578186297664</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>270.36033333333336</v>
+      </c>
+      <c r="C27">
+        <v>0.14036289873221952</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>292.90933333333334</v>
+      </c>
+      <c r="C28">
+        <v>0.14081543897531107</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>313.00833333333333</v>
+      </c>
+      <c r="C29">
+        <v>0.14126797921840262</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>331.63533333333334</v>
+      </c>
+      <c r="C30">
+        <v>0.14096628572300826</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>351.24333333333334</v>
+      </c>
+      <c r="C31">
+        <v>0.1406645922276139</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>368.89033333333333</v>
+      </c>
+      <c r="C32">
+        <v>0.14111713247070545</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>381.14533333333333</v>
+      </c>
+      <c r="C33">
+        <v>0.14111713247070545</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>399.28233333333333</v>
+      </c>
+      <c r="C34">
+        <v>0.14156967271379695</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added calculation of coefficients a0, a1 and c0
</commit_message>
<xml_diff>
--- a/Ag_kinetics.xlsx
+++ b/Ag_kinetics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luise\iCloudDrive\Ennova\P&amp;A kinetics tuning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9793F7-2596-4196-803D-604A0A3961B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B2DCCE-E8C4-4D2B-A44D-D3E0A434CAD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{85EE5AE4-3DA7-4426-97B8-6903418DBB70}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{85EE5AE4-3DA7-4426-97B8-6903418DBB70}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="2" r:id="rId1"/>
@@ -442,7 +442,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -497,7 +497,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -820,7 +819,7 @@
   </sheetPr>
   <dimension ref="B1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
@@ -880,15 +879,15 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
       <c r="J7" s="23"/>
-      <c r="K7" s="25" t="s">
+      <c r="K7" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="25"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="24"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
@@ -981,7 +980,7 @@
         <v>15.670998837890844</v>
       </c>
       <c r="O9" s="16"/>
-      <c r="P9" s="24">
+      <c r="P9">
         <v>22.88926523648297</v>
       </c>
       <c r="Q9" s="12">
@@ -1028,7 +1027,7 @@
       <c r="N10">
         <v>15.816842058526548</v>
       </c>
-      <c r="P10" s="24">
+      <c r="P10">
         <v>22.889265236484007</v>
       </c>
       <c r="Q10" s="12">
@@ -1075,7 +1074,7 @@
       <c r="N11">
         <v>15.97057978082789</v>
       </c>
-      <c r="P11" s="24">
+      <c r="P11">
         <v>22.889265236484007</v>
       </c>
       <c r="Q11" s="12">
@@ -1122,7 +1121,7 @@
       <c r="N12">
         <v>15.038418494274167</v>
       </c>
-      <c r="P12" s="24">
+      <c r="P12">
         <v>22.349547063064552</v>
       </c>
       <c r="Q12" s="12">
@@ -1169,7 +1168,7 @@
       <c r="N13">
         <v>15.227161798036935</v>
       </c>
-      <c r="P13" s="24">
+      <c r="P13">
         <v>22.349547063064552</v>
       </c>
       <c r="Q13" s="12">
@@ -1216,7 +1215,7 @@
       <c r="N14">
         <v>15.563012107976123</v>
       </c>
-      <c r="P14" s="24">
+      <c r="P14">
         <v>22.349547063064552</v>
       </c>
       <c r="Q14" s="12">
@@ -1235,7 +1234,6 @@
       <c r="I15" s="19"/>
       <c r="J15" s="12"/>
       <c r="K15" s="11"/>
-      <c r="P15" s="24"/>
       <c r="Q15" s="12"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
@@ -1250,7 +1248,6 @@
       <c r="I16" s="19"/>
       <c r="J16" s="12"/>
       <c r="K16" s="11"/>
-      <c r="P16" s="24"/>
       <c r="Q16" s="12"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.3">
@@ -1265,7 +1262,6 @@
       <c r="I17" s="19"/>
       <c r="J17" s="12"/>
       <c r="K17" s="11"/>
-      <c r="P17" s="24"/>
       <c r="Q17" s="12"/>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.3">
@@ -1654,8 +1650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38A111BB-A23C-48E8-9875-888A70D3D01B}">
   <dimension ref="B1:C38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D1:D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1702,7 +1698,7 @@
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6">
-        <v>2.7151000000000001</v>
+        <v>2.9</v>
       </c>
       <c r="C6">
         <v>4.7728429394167389E-2</v>

</xml_diff>

<commit_message>
Fixed ca0 not defined error
</commit_message>
<xml_diff>
--- a/Ag_kinetics.xlsx
+++ b/Ag_kinetics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luise\iCloudDrive\Ennova\P&amp;A kinetics tuning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B2DCCE-E8C4-4D2B-A44D-D3E0A434CAD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349A8888-5A31-457E-8C51-EE086D29EF66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{85EE5AE4-3DA7-4426-97B8-6903418DBB70}"/>
   </bookViews>
@@ -232,9 +232,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -258,18 +255,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -442,17 +433,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -461,7 +451,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -476,28 +466,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -872,105 +862,105 @@
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="24" t="s">
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="24"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="M8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="N8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="O8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="P8" s="4" t="s">
+      <c r="P8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="Q8" s="5" t="s">
+      <c r="Q8" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>1</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="10">
         <v>104</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="11">
         <v>1</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="F9" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="18" t="s">
         <v>33</v>
       </c>
       <c r="H9">
         <v>75</v>
       </c>
-      <c r="I9" s="19" t="s">
+      <c r="I9" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="12">
+      <c r="J9" s="11">
         <v>55</v>
       </c>
       <c r="K9">
         <v>0.85828150950348459</v>
       </c>
-      <c r="L9" s="16">
+      <c r="L9" s="15">
         <v>0.48585024167655921</v>
       </c>
       <c r="M9">
@@ -979,40 +969,40 @@
       <c r="N9">
         <v>15.670998837890844</v>
       </c>
-      <c r="O9" s="16"/>
+      <c r="O9" s="15"/>
       <c r="P9">
         <v>22.88926523648297</v>
       </c>
-      <c r="Q9" s="12">
+      <c r="Q9" s="11">
         <v>14.7525019671374</v>
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B10" s="9">
+      <c r="B10" s="8">
         <v>2</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="10">
         <v>104</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="11">
         <v>1</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="18" t="s">
         <v>33</v>
       </c>
       <c r="H10">
         <v>75</v>
       </c>
-      <c r="I10" s="19" t="s">
+      <c r="I10" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="J10" s="12">
+      <c r="J10" s="11">
         <v>60</v>
       </c>
       <c r="K10">
@@ -1030,36 +1020,36 @@
       <c r="P10">
         <v>22.889265236484007</v>
       </c>
-      <c r="Q10" s="12">
+      <c r="Q10" s="11">
         <v>13.569999722793746</v>
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B11" s="9">
+      <c r="B11" s="8">
         <v>3</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="10">
         <v>104</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="11">
         <v>1</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="18" t="s">
         <v>33</v>
       </c>
       <c r="H11">
         <v>75</v>
       </c>
-      <c r="I11" s="19" t="s">
+      <c r="I11" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="11">
         <v>60</v>
       </c>
       <c r="K11">
@@ -1077,36 +1067,36 @@
       <c r="P11">
         <v>22.889265236484007</v>
       </c>
-      <c r="Q11" s="12">
+      <c r="Q11" s="11">
         <v>13.84644984127668</v>
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="9">
+      <c r="B12" s="8">
         <v>4</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="10">
         <v>176</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="11">
         <v>1</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="18" t="s">
         <v>33</v>
       </c>
       <c r="H12">
         <v>75</v>
       </c>
-      <c r="I12" s="19" t="s">
+      <c r="I12" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="J12" s="12">
+      <c r="J12" s="11">
         <v>62</v>
       </c>
       <c r="K12">
@@ -1124,36 +1114,36 @@
       <c r="P12">
         <v>22.349547063064552</v>
       </c>
-      <c r="Q12" s="12">
+      <c r="Q12" s="11">
         <v>12.466964632001005</v>
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B13" s="9">
+      <c r="B13" s="8">
         <v>5</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="10">
         <v>176</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="11">
         <v>1</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="G13" s="18" t="s">
         <v>33</v>
       </c>
       <c r="H13">
         <v>75</v>
       </c>
-      <c r="I13" s="19" t="s">
+      <c r="I13" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="J13" s="12">
+      <c r="J13" s="11">
         <v>62</v>
       </c>
       <c r="K13">
@@ -1171,36 +1161,36 @@
       <c r="P13">
         <v>22.349547063064552</v>
       </c>
-      <c r="Q13" s="12">
+      <c r="Q13" s="11">
         <v>12.760943525221411</v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B14" s="9">
+      <c r="B14" s="8">
         <v>6</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="10">
         <v>176</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="11">
         <v>1</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="18" t="s">
         <v>33</v>
       </c>
       <c r="H14">
         <v>75</v>
       </c>
-      <c r="I14" s="19" t="s">
+      <c r="I14" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="J14" s="12">
+      <c r="J14" s="11">
         <v>62</v>
       </c>
       <c r="K14">
@@ -1218,71 +1208,71 @@
       <c r="P14">
         <v>22.349547063064552</v>
       </c>
-      <c r="Q14" s="12">
+      <c r="Q14" s="11">
         <v>13.284010695462358</v>
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B15" s="9">
+      <c r="B15" s="8">
         <v>7</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="11"/>
-      <c r="Q15" s="12"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="10"/>
+      <c r="Q15" s="11"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B16" s="9">
+      <c r="B16" s="8">
         <v>8</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="11"/>
-      <c r="Q16" s="12"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="10"/>
+      <c r="Q16" s="11"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B17" s="9">
+      <c r="B17" s="8">
         <v>9</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="11"/>
-      <c r="Q17" s="12"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="10"/>
+      <c r="Q17" s="11"/>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B18" s="10">
+      <c r="B18" s="9">
         <v>10</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="14"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1651,7 +1641,7 @@
   <dimension ref="B1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1698,7 +1688,7 @@
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6">
-        <v>2.9</v>
+        <v>2.7151000000000001</v>
       </c>
       <c r="C6">
         <v>4.7728429394167389E-2</v>
@@ -1970,7 +1960,7 @@
   <dimension ref="B1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D1:D2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1987,7 +1977,7 @@
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>0</v>
       </c>
     </row>
@@ -1995,7 +1985,7 @@
       <c r="B3">
         <v>0.505</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>6.9062154215709208E-3</v>
       </c>
     </row>
@@ -2003,7 +1993,7 @@
       <c r="B4">
         <v>2.02</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>1.3171647968975487E-2</v>
       </c>
     </row>
@@ -2011,7 +2001,7 @@
       <c r="B5">
         <v>3.03</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>1.844030715656567E-2</v>
       </c>
     </row>
@@ -2019,7 +2009,7 @@
       <c r="B6">
         <v>4.04</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>2.5773711160914176E-2</v>
       </c>
     </row>
@@ -2027,7 +2017,7 @@
       <c r="B7">
         <v>5.556</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7">
         <v>3.2751124679614697E-2</v>
       </c>
     </row>
@@ -2035,7 +2025,7 @@
       <c r="B8">
         <v>7.0709999999999997</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8">
         <v>3.8660566741371277E-2</v>
       </c>
     </row>
@@ -2043,7 +2033,7 @@
       <c r="B9">
         <v>9.0909999999999993</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9">
         <v>4.5637980260071806E-2</v>
       </c>
     </row>
@@ -2051,7 +2041,7 @@
       <c r="B10">
         <v>10.606</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10">
         <v>5.1618620418957963E-2</v>
       </c>
     </row>
@@ -2059,7 +2049,7 @@
       <c r="B11">
         <v>13.635999999999999</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11">
         <v>5.7884052966362516E-2</v>
       </c>
     </row>
@@ -2067,7 +2057,7 @@
       <c r="B12">
         <v>15.151999999999999</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12">
         <v>6.4505475999415043E-2</v>
       </c>
     </row>
@@ -2075,7 +2065,7 @@
       <c r="B13">
         <v>20.202000000000002</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13">
         <v>7.4330813403299445E-2</v>
       </c>
     </row>
@@ -2083,7 +2073,7 @@
       <c r="B14">
         <v>25.253</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14">
         <v>8.408495271005427E-2</v>
       </c>
     </row>
@@ -2091,7 +2081,7 @@
       <c r="B15">
         <v>30.808</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15">
         <v>9.1133564325884389E-2</v>
       </c>
     </row>
@@ -2099,7 +2089,7 @@
       <c r="B16">
         <v>39.899000000000001</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16">
         <v>0.10337963703217513</v>
       </c>
     </row>
@@ -2107,7 +2097,7 @@
       <c r="B17">
         <v>48.99</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17">
         <v>0.11000106006522765</v>
       </c>
     </row>
@@ -2115,7 +2105,7 @@
       <c r="B18">
         <v>58.081000000000003</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18">
         <v>0.11669368119540977</v>
       </c>
     </row>
@@ -2123,7 +2113,7 @@
       <c r="B19">
         <v>70.706999999999994</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19">
         <v>0.12367109471411034</v>
       </c>
     </row>
@@ -2131,7 +2121,7 @@
       <c r="B20">
         <v>85.858999999999995</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20">
         <v>0.12972293297012608</v>
       </c>
     </row>
@@ -2139,7 +2129,7 @@
       <c r="B21">
         <v>103.03</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21">
         <v>0.13427961118642032</v>
       </c>
     </row>
@@ -2147,7 +2137,7 @@
       <c r="B22">
         <v>123.232</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22">
         <v>0.13855149701419608</v>
       </c>
     </row>
@@ -2155,7 +2145,7 @@
       <c r="B23">
         <v>148.99</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23">
         <v>0.14282338284197191</v>
       </c>
     </row>
@@ -2163,7 +2153,7 @@
       <c r="B24">
         <v>176.26300000000001</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24">
         <v>0.14467453336734148</v>
       </c>
     </row>
@@ -2171,7 +2161,7 @@
       <c r="B25">
         <v>209.596</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25">
         <v>0.14759365534965496</v>
       </c>
     </row>
@@ -2179,7 +2169,7 @@
       <c r="B26">
         <v>226.768</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26">
         <v>0.14866162680659895</v>
       </c>
     </row>
@@ -2187,7 +2177,7 @@
       <c r="B27">
         <v>250.505</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27">
         <v>0.14944480587502448</v>
       </c>
     </row>
@@ -2195,7 +2185,7 @@
       <c r="B28">
         <v>273.73700000000002</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28">
         <v>0.14987199445780205</v>
       </c>
     </row>
@@ -2203,7 +2193,7 @@
       <c r="B29">
         <v>303.02999999999997</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29">
         <v>0.15101116401187561</v>
       </c>
     </row>
@@ -2211,7 +2201,7 @@
       <c r="B30">
         <v>321.71699999999998</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30">
         <v>0.15143835259465319</v>
       </c>
     </row>
@@ -2219,7 +2209,7 @@
       <c r="B31">
         <v>340.90899999999999</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31">
         <v>0.15186554117743081</v>
       </c>
     </row>
@@ -2227,7 +2217,7 @@
       <c r="B32">
         <v>357.57600000000002</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32">
         <v>0.15158074878891237</v>
       </c>
     </row>
@@ -2235,7 +2225,7 @@
       <c r="B33">
         <v>371.71699999999998</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33">
         <v>0.151651946886042</v>
       </c>
     </row>
@@ -2243,7 +2233,7 @@
       <c r="B34">
         <v>389.39400000000001</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34">
         <v>0.15172314498317158</v>
       </c>
     </row>
@@ -2251,7 +2241,7 @@
       <c r="B35">
         <v>397.47500000000002</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35">
         <v>0.15136715449752361</v>
       </c>
     </row>

</xml_diff>